<commit_message>
xmlUtil > addTest with class method.
</commit_message>
<xml_diff>
--- a/src/test/resources/testng-config.xlsx
+++ b/src/test/resources/testng-config.xlsx
@@ -6,88 +6,127 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Groups" sheetId="1" r:id="rId4"/>
-    <sheet name="Classes" sheetId="2" r:id="rId5"/>
+    <sheet name="Classes" sheetId="1" r:id="rId4"/>
+    <sheet name="Groups" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>ClassName</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>Smoke Test</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>ClassName1</t>
+  </si>
+  <si>
+    <t>com.changan.testcase.ai</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>ClassName2</t>
+  </si>
+  <si>
+    <t>com.changan.testcase.cloud</t>
+  </si>
+  <si>
+    <t>ClassName3</t>
+  </si>
+  <si>
+    <t>Golden Test</t>
+  </si>
+  <si>
+    <t>ClassName5</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Regression Test</t>
+  </si>
+  <si>
+    <t>ClassName6</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>com.changan.testcase.finance</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>ClassSprint1-1</t>
+  </si>
+  <si>
+    <t>ClassSprint1-2</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>ClassSprint2-1</t>
+  </si>
+  <si>
+    <t>ClassSprint2-2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>ClassSprint3-1</t>
+  </si>
+  <si>
+    <t>ClassSprint3-2</t>
+  </si>
+  <si>
+    <t>ClassSprint3-3</t>
+  </si>
   <si>
     <t>GroupName</t>
   </si>
   <si>
-    <t>TestName</t>
-  </si>
-  <si>
-    <t>Flag</t>
-  </si>
-  <si>
     <t>G1</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>G2</t>
   </si>
   <si>
     <t>G3</t>
   </si>
   <si>
-    <t>T2</t>
-  </si>
-  <si>
     <t>G4</t>
   </si>
   <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>G5</t>
   </si>
   <si>
     <t>G6</t>
-  </si>
-  <si>
-    <t>ClassName</t>
-  </si>
-  <si>
-    <t>Package</t>
-  </si>
-  <si>
-    <t>ClassName1</t>
-  </si>
-  <si>
-    <t>com.changan.testcase.module1</t>
-  </si>
-  <si>
-    <t>ClassName2</t>
-  </si>
-  <si>
-    <t>ClassName3</t>
-  </si>
-  <si>
-    <t>com.changan.testcase.module2</t>
-  </si>
-  <si>
-    <t>ClassName4</t>
-  </si>
-  <si>
-    <t>ClassName5</t>
-  </si>
-  <si>
-    <t>com.changan.testcase.module3</t>
-  </si>
-  <si>
-    <t>ClassName6</t>
   </si>
 </sst>
 </file>
@@ -146,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -174,6 +213,36 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -207,7 +276,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -249,13 +318,105 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="14"/>
       </bottom>
       <diagonal/>
     </border>
@@ -265,7 +426,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -275,16 +436,43 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -293,25 +481,40 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -334,8 +537,9 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1400,7 +1604,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1409,7 +1613,10 @@
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.9062" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
+    <col min="7" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1422,105 +1629,286 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" ht="32.25" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="B2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="7">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s" s="8">
+      <c r="C2" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" ht="32.05" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="B3" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="11">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="8">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s" s="16">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="D5" t="s" s="12">
         <v>8</v>
       </c>
-      <c r="C4" t="s" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="6">
+      <c r="E5" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" ht="32.05" customHeight="1">
+      <c r="A6" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s" s="16">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" ht="32.05" customHeight="1">
+      <c r="A7" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s" s="16">
         <v>10</v>
       </c>
-      <c r="C5" t="s" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="C7" t="s" s="18">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s" s="6">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s" s="12">
         <v>12</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="E8" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s" s="17">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s" s="11">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s" s="19">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" t="s" s="13">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="C6" t="s" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s" s="7">
+      <c r="C12" t="s" s="11">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" t="s" s="13">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="C7" t="s" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
+      <c r="C13" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="20">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s" s="11">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="F16" s="14"/>
     </row>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -1533,148 +1921,155 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="12" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="12" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="12" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="12" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="12" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="21" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="21" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="21" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="21" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="21" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="8">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" t="s" s="13">
         <v>14</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" ht="32.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B4" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="B2" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" ht="32.05" customHeight="1">
-      <c r="A3" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s" s="8">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" ht="32.05" customHeight="1">
-      <c r="A4" t="s" s="6">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" t="s" s="15">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" t="s" s="15">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s" s="8">
-        <v>11</v>
-      </c>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" ht="32.05" customHeight="1">
-      <c r="A7" t="s" s="15">
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="B7" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s" s="8">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="E7" s="11"/>
+      <c r="B6" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="13">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
     </row>
   </sheetData>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>

<commit_message>
add getTestClassandGroups, next step generate the testng.xml by the test info.
</commit_message>
<xml_diff>
--- a/src/test/resources/testng-config.xlsx
+++ b/src/test/resources/testng-config.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId4"/>
     <sheet name="Groups" sheetId="2" r:id="rId5"/>
+    <sheet name="CheckConfig" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>TestName</t>
   </si>
@@ -127,6 +128,27 @@
   </si>
   <si>
     <t>G6</t>
+  </si>
+  <si>
+    <t>表格 1</t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>同一个test下面不能有重复的class</t>
+  </si>
+  <si>
+    <t>testname和classname不能为空</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>同一个test下面不能有重复的group</t>
+  </si>
+  <si>
+    <t>testname和groupname不能为空</t>
   </si>
 </sst>
 </file>
@@ -159,7 +181,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +206,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -420,13 +454,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -505,16 +644,46 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -540,6 +709,10 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1613,7 +1786,7 @@
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.9062" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
     <col min="7" max="256" width="16.3516" style="1" customWidth="1"/>
@@ -1921,7 +2094,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2023,50 +2196,8 @@
       <c r="C7" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2075,4 +2206,135 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="28" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="28" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="28" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="28" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="28" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18" customHeight="1">
+      <c r="A1" t="s" s="29">
+        <v>38</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" ht="30.6" customHeight="1">
+      <c r="A4" t="s" s="34">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s" s="35">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s" s="36">
+        <v>41</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+    </row>
+    <row r="5" ht="30.6" customHeight="1">
+      <c r="A5" t="s" s="34">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s" s="35">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s" s="36">
+        <v>44</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+    </row>
+    <row r="6" ht="14.05" customHeight="1">
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+    </row>
+    <row r="7" ht="14.05" customHeight="1">
+      <c r="A7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+    </row>
+    <row r="8" ht="14.05" customHeight="1">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+    </row>
+    <row r="9" ht="14.05" customHeight="1">
+      <c r="A9" s="38"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+    </row>
+    <row r="10" ht="14.05" customHeight="1">
+      <c r="A10" s="38"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+    </row>
+    <row r="11" ht="14.05" customHeight="1">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+    </row>
+    <row r="12" ht="14.05" customHeight="1">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
integrate the extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/testng-config.xlsx
+++ b/src/test/resources/testng-config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>TestName</t>
   </si>
@@ -31,105 +31,24 @@
     <t>Flag</t>
   </si>
   <si>
-    <t>Smoke Test</t>
-  </si>
-  <si>
-    <t>AI</t>
-  </si>
-  <si>
-    <t>ClassName1</t>
-  </si>
-  <si>
-    <t>com.changan.testcase.ai</t>
+    <t>Regression Test</t>
+  </si>
+  <si>
+    <t>ShopClient</t>
+  </si>
+  <si>
+    <t>TC001_ShopClient_VerifyLogin</t>
+  </si>
+  <si>
+    <t>com.changan.testcases.shopclient</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Cloud</t>
-  </si>
-  <si>
-    <t>ClassName2</t>
-  </si>
-  <si>
-    <t>com.changan.testcase.cloud</t>
-  </si>
-  <si>
-    <t>ClassName3</t>
-  </si>
-  <si>
-    <t>Golden Test</t>
-  </si>
-  <si>
-    <t>ClassName5</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Regression Test</t>
-  </si>
-  <si>
-    <t>ClassName6</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>com.changan.testcase.finance</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>ClassSprint1-1</t>
-  </si>
-  <si>
-    <t>ClassSprint1-2</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>ClassSprint2-1</t>
-  </si>
-  <si>
-    <t>ClassSprint2-2</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>ClassSprint3-1</t>
-  </si>
-  <si>
-    <t>ClassSprint3-2</t>
-  </si>
-  <si>
-    <t>ClassSprint3-3</t>
-  </si>
-  <si>
     <t>GroupName</t>
   </si>
   <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
-    <t>G5</t>
-  </si>
-  <si>
-    <t>G6</t>
-  </si>
-  <si>
     <t>表格 1</t>
   </si>
   <si>
@@ -149,6 +68,9 @@
   </si>
   <si>
     <t>testname和groupname不能为空</t>
+  </si>
+  <si>
+    <t>两个sheet不能有多余的空行</t>
   </si>
 </sst>
 </file>
@@ -158,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -180,8 +102,13 @@
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="13"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,30 +123,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="18"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -238,7 +153,7 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -247,25 +162,25 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -277,178 +192,11 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="14"/>
       </bottom>
@@ -456,106 +204,109 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="16"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="15"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="15"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="16"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="17"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="16"/>
-      </left>
-      <right style="thin">
-        <color indexed="16"/>
-      </right>
-      <top style="thin">
-        <color indexed="16"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -565,7 +316,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -578,112 +329,64 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -705,14 +408,11 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa9b6c6"/>
+      <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1777,7 +1477,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1810,7 +1510,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" ht="32.25" customHeight="1">
+    <row r="2" ht="20.05" customHeight="1">
       <c r="A2" t="s" s="4">
         <v>5</v>
       </c>
@@ -1823,262 +1523,10 @@
       <c r="D2" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="8">
+      <c r="E2" t="s" s="4">
         <v>9</v>
       </c>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" ht="32.05" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" ht="32.05" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" t="s" s="13">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="16">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" t="s" s="13">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s" s="16">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" ht="32.05" customHeight="1">
-      <c r="A7" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s" s="16">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s" s="18">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s" s="6">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="13">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s" s="19">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="13">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="13">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s" s="11">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="13">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s" s="10">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s" s="11">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s" s="11">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s" s="11">
-        <v>30</v>
-      </c>
-      <c r="D16" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="F16" s="14"/>
+      <c r="F2" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -2094,110 +1542,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="21" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="21" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="21" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="21" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="21" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="21" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="9" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="10">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s" s="2">
+      <c r="B1" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s" s="5">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="13">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="13">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="13">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="13">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2213,119 +1583,119 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="28" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="28" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="28" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="28" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="28" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="28" customWidth="1"/>
+    <col min="1" max="1" width="40.7266" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="13" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="13" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="13" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="13" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
-      <c r="A1" t="s" s="29">
-        <v>38</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="A1" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" ht="30.6" customHeight="1">
-      <c r="A4" t="s" s="34">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s" s="35">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s" s="36">
-        <v>41</v>
-      </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="A4" t="s" s="21">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="30.6" customHeight="1">
-      <c r="A5" t="s" s="34">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s" s="35">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s" s="36">
-        <v>44</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
+      <c r="A5" t="s" s="21">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="A6" t="s" s="21">
+        <v>18</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="38"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" ht="14.05" customHeight="1">
-      <c r="A9" s="38"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" ht="14.05" customHeight="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" ht="14.05" customHeight="1">
-      <c r="A12" s="38"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add two test cases for demo
</commit_message>
<xml_diff>
--- a/src/test/resources/testng-config.xlsx
+++ b/src/test/resources/testng-config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>TestName</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>TC002_ShopClient_VerifyRegPageTitle</t>
   </si>
   <si>
     <t>GroupName</t>
@@ -80,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -106,6 +109,11 @@
       <sz val="9"/>
       <color indexed="13"/>
       <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="15"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="5">
@@ -134,7 +142,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -192,6 +200,47 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
@@ -208,33 +257,33 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -245,7 +294,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -255,10 +304,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -316,7 +365,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -344,40 +393,49 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -412,6 +470,7 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffa9b6c6"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffa9b6c6"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -1477,7 +1536,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1527,6 +1586,24 @@
         <v>9</v>
       </c>
       <c r="F2" s="8"/>
+    </row>
+    <row r="3" ht="26.7" customHeight="1">
+      <c r="A3" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="F3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -1548,26 +1625,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="9" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="9" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="12" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="12" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="12" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="10">
+      <c r="A1" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s" s="10">
+      <c r="B1" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s" s="13">
         <v>4</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -1589,110 +1666,110 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="40.7266" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="13" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="13" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="13" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="13" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="1" width="40.6719" style="16" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="16" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="16" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="16" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
-      <c r="A1" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
+      <c r="A1" t="s" s="17">
+        <v>12</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" ht="30.6" customHeight="1">
-      <c r="A4" t="s" s="21">
-        <v>12</v>
+      <c r="A4" t="s" s="24">
+        <v>13</v>
       </c>
       <c r="B4" t="s" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" ht="30.6" customHeight="1">
-      <c r="A5" t="s" s="21">
-        <v>15</v>
+      <c r="A5" t="s" s="24">
+        <v>16</v>
       </c>
       <c r="B5" t="s" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" t="s" s="21">
-        <v>18</v>
-      </c>
-      <c r="B6" s="22"/>
+      <c r="A6" t="s" s="24">
+        <v>19</v>
+      </c>
+      <c r="B6" s="25"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" ht="14.05" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" ht="14.05" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" ht="14.05" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>

</xml_diff>